<commit_message>
Separated register function in separate file
</commit_message>
<xml_diff>
--- a/Registration files/Registered_users.xlsx
+++ b/Registration files/Registered_users.xlsx
@@ -466,7 +466,7 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>Ikki Maru</t>
+          <t>Ikki ikkov</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
@@ -476,7 +476,7 @@
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>qwer@mail.ru</t>
+          <t>asdads@mail.com</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">

</xml_diff>

<commit_message>
Distributed to different files, from monolith to routers,utils and handlers
</commit_message>
<xml_diff>
--- a/Registration files/Registered_users.xlsx
+++ b/Registration files/Registered_users.xlsx
@@ -466,7 +466,7 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>Ikki ikkov</t>
+          <t>Gul gul</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
@@ -476,7 +476,7 @@
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>asdads@mail.com</t>
+          <t>ewrwe@gmail.ru</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">

</xml_diff>

<commit_message>
Made a request by broadcast to check if admin could make newslettering by web
</commit_message>
<xml_diff>
--- a/Registration files/Registered_users.xlsx
+++ b/Registration files/Registered_users.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E3"/>
+  <dimension ref="A1:E4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -492,10 +492,8 @@
           <t>Saidov Khushdil</t>
         </is>
       </c>
-      <c r="C3" t="inlineStr">
-        <is>
-          <t>79177131361</t>
-        </is>
+      <c r="C3" t="n">
+        <v>79177131361</v>
       </c>
       <c r="D3" t="inlineStr">
         <is>
@@ -505,6 +503,31 @@
       <c r="E3" t="inlineStr">
         <is>
           <t>xuwdil None</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="n">
+        <v>974794263</v>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>Головач Лена</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>+992938636344</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>golovach@lena.ker</t>
+        </is>
+      </c>
+      <c r="E4" t="inlineStr">
+        <is>
+          <t>Buzurgmehr Abdulloev</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Added buttons for TDH(Test Drive History) and SH(Service History)
</commit_message>
<xml_diff>
--- a/Registration files/Registered_users.xlsx
+++ b/Registration files/Registered_users.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F2"/>
+  <dimension ref="A1:F4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -467,29 +467,85 @@
     </row>
     <row r="2">
       <c r="A2" t="n">
+        <v>5547528084</v>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>Хушдил Саидов</t>
+        </is>
+      </c>
+      <c r="C2" t="n">
+        <v>79177131361</v>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>xuwdi@mail.ru</t>
+        </is>
+      </c>
+      <c r="E2" t="inlineStr">
+        <is>
+          <t>xuwdil None</t>
+        </is>
+      </c>
+      <c r="F2" t="inlineStr">
+        <is>
+          <t>RU</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="n">
         <v>631886740</v>
       </c>
-      <c r="B2" t="inlineStr">
-        <is>
-          <t>Woaw woaw</t>
-        </is>
-      </c>
-      <c r="C2" t="n">
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>Ikki maru</t>
+        </is>
+      </c>
+      <c r="C3" t="n">
         <v>992907510905</v>
       </c>
-      <c r="D2" t="inlineStr">
-        <is>
-          <t>new_email@mail.ru</t>
-        </is>
-      </c>
-      <c r="E2" t="inlineStr">
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>ikki@maru.com</t>
+        </is>
+      </c>
+      <c r="E3" t="inlineStr">
         <is>
           <t>Ismat .</t>
         </is>
       </c>
-      <c r="F2" t="inlineStr">
+      <c r="F3" t="inlineStr">
         <is>
           <t>EN</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="n">
+        <v>974794263</v>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>Гульдартабакова Гульдартабакнукрахуросонабегим</t>
+        </is>
+      </c>
+      <c r="C4" t="n">
+        <v>992938636344</v>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>thesarboz@gmail.com</t>
+        </is>
+      </c>
+      <c r="E4" t="inlineStr">
+        <is>
+          <t>Buzurgmehr Abdulloev</t>
+        </is>
+      </c>
+      <c r="F4" t="inlineStr">
+        <is>
+          <t>RU</t>
         </is>
       </c>
     </row>

</xml_diff>